<commit_message>
Compared different batch sizes
</commit_message>
<xml_diff>
--- a/Pytorch/Results/Structure.xlsx
+++ b/Pytorch/Results/Structure.xlsx
@@ -61,12 +61,6 @@
     <t>lr=0.1</t>
   </si>
   <si>
-    <t>lr=0.01/0.1</t>
-  </si>
-  <si>
-    <t>lr=0.01/3</t>
-  </si>
-  <si>
     <t>lr=1</t>
   </si>
   <si>
@@ -74,15 +68,6 @@
   </si>
   <si>
     <t>lr=0.001</t>
-  </si>
-  <si>
-    <t>lr=0.001/0.01</t>
-  </si>
-  <si>
-    <t>lr=0.001/0.1</t>
-  </si>
-  <si>
-    <t>lr=0.001/1</t>
   </si>
   <si>
     <t>CIFAR100</t>
@@ -167,6 +152,21 @@
   <si>
     <t>find best
 decay-type for constant LR</t>
+  </si>
+  <si>
+    <t>lr=0.01-0.1</t>
+  </si>
+  <si>
+    <t>lr=0.01-3</t>
+  </si>
+  <si>
+    <t>lr=0.001-0.01</t>
+  </si>
+  <si>
+    <t>lr=0.001-0.1</t>
+  </si>
+  <si>
+    <t>lr=0.001-1</t>
   </si>
 </sst>
 </file>
@@ -390,6 +390,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -399,14 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -415,9 +418,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,8 +726,8 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,37 +744,37 @@
     <col min="10" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:11" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="G1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="22">
+      <c r="H1" s="16">
         <f>SUM(H2:H101)</f>
-        <v>1</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>41</v>
+        <v>4</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -797,16 +797,16 @@
         <v>13</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>42</v>
+        <v>1</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
@@ -819,13 +819,13 @@
         <v>13</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
@@ -837,13 +837,13 @@
         <v>13</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="20"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5"/>
@@ -855,13 +855,13 @@
         <v>13</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="21"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
@@ -873,12 +873,12 @@
         <v>14</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H6" s="3">
         <v>0</v>
       </c>
-      <c r="I6" s="13"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
@@ -887,15 +887,15 @@
       <c r="D7" s="8"/>
       <c r="E7" s="1"/>
       <c r="F7" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H7" s="3">
         <v>0</v>
       </c>
-      <c r="I7" s="13"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
@@ -909,12 +909,12 @@
         <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H8" s="3">
         <v>0</v>
       </c>
-      <c r="I8" s="13"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
@@ -926,12 +926,12 @@
         <v>14</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H9" s="3">
         <v>0</v>
       </c>
-      <c r="I9" s="13"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="5"/>
@@ -940,37 +940,37 @@
       <c r="D10" s="8"/>
       <c r="E10" s="1"/>
       <c r="F10" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H10" s="3">
         <v>0</v>
       </c>
-      <c r="I10" s="14"/>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H11" s="3">
         <v>0</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>44</v>
+      <c r="I11" s="17" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
@@ -980,15 +980,15 @@
       <c r="D12" s="8"/>
       <c r="E12" s="1"/>
       <c r="F12" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H12" s="3">
         <v>0</v>
       </c>
-      <c r="I12" s="13"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
@@ -999,15 +999,15 @@
         <v>9</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H13" s="3">
         <v>0</v>
       </c>
-      <c r="I13" s="13"/>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
@@ -1016,15 +1016,15 @@
       <c r="D14" s="8"/>
       <c r="E14" s="1"/>
       <c r="F14" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H14" s="3">
         <v>0</v>
       </c>
-      <c r="I14" s="13"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
@@ -1035,15 +1035,15 @@
         <v>10</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H15" s="3">
         <v>0</v>
       </c>
-      <c r="I15" s="13"/>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
@@ -1052,37 +1052,37 @@
       <c r="D16" s="8"/>
       <c r="E16" s="1"/>
       <c r="F16" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H16" s="3">
         <v>0</v>
       </c>
-      <c r="I16" s="14"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H17" s="3">
         <v>0</v>
       </c>
-      <c r="I17" s="12" t="s">
-        <v>45</v>
+      <c r="I17" s="17" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
@@ -1092,15 +1092,15 @@
       <c r="D18" s="8"/>
       <c r="E18" s="1"/>
       <c r="F18" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H18" s="3">
         <v>0</v>
       </c>
-      <c r="I18" s="13"/>
+      <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
@@ -1111,15 +1111,15 @@
         <v>9</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H19" s="3">
         <v>0</v>
       </c>
-      <c r="I19" s="13"/>
+      <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
@@ -1128,15 +1128,15 @@
       <c r="D20" s="8"/>
       <c r="E20" s="1"/>
       <c r="F20" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H20" s="3">
         <v>0</v>
       </c>
-      <c r="I20" s="13"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
@@ -1147,15 +1147,15 @@
         <v>10</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H21" s="3">
         <v>0</v>
       </c>
-      <c r="I21" s="13"/>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5"/>
@@ -1164,37 +1164,37 @@
       <c r="D22" s="8"/>
       <c r="E22" s="1"/>
       <c r="F22" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
       </c>
-      <c r="I22" s="14"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
       </c>
-      <c r="I23" s="12" t="s">
-        <v>46</v>
+      <c r="I23" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
@@ -1204,15 +1204,15 @@
       <c r="D24" s="8"/>
       <c r="E24" s="1"/>
       <c r="F24" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
       </c>
-      <c r="I24" s="13"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
@@ -1223,15 +1223,15 @@
         <v>9</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H25" s="3">
         <v>0</v>
       </c>
-      <c r="I25" s="13"/>
+      <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -1240,15 +1240,15 @@
       <c r="D26" s="8"/>
       <c r="E26" s="1"/>
       <c r="F26" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
       </c>
-      <c r="I26" s="13"/>
+      <c r="I26" s="18"/>
     </row>
     <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
@@ -1259,15 +1259,15 @@
         <v>10</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H27" s="3">
         <v>0</v>
       </c>
-      <c r="I27" s="13"/>
+      <c r="I27" s="18"/>
     </row>
     <row r="28" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5"/>
@@ -1276,15 +1276,15 @@
       <c r="D28" s="8"/>
       <c r="E28" s="1"/>
       <c r="F28" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H28" s="3">
         <v>0</v>
       </c>
-      <c r="I28" s="14"/>
+      <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
@@ -1299,10 +1299,10 @@
         <v>7</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H29" s="3">
         <v>0</v>
@@ -1318,7 +1318,7 @@
         <v>13</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H30" s="3">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>14</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H31" s="3">
         <v>0</v>
@@ -1347,10 +1347,10 @@
       <c r="D32" s="8"/>
       <c r="E32" s="1"/>
       <c r="F32" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H32" s="3">
         <v>0</v>
@@ -1361,22 +1361,22 @@
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H33" s="3">
         <v>0</v>
       </c>
-      <c r="I33" s="12" t="s">
-        <v>43</v>
+      <c r="I33" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
@@ -1386,15 +1386,15 @@
       <c r="D34" s="8"/>
       <c r="E34" s="1"/>
       <c r="F34" s="9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H34" s="3">
         <v>0</v>
       </c>
-      <c r="I34" s="13"/>
+      <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
@@ -1403,36 +1403,36 @@
       <c r="D35" s="8"/>
       <c r="E35" s="1"/>
       <c r="F35" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H35" s="3">
         <v>0</v>
       </c>
-      <c r="I35" s="13"/>
+      <c r="I35" s="18"/>
     </row>
     <row r="36" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H36" s="3">
         <v>0</v>
       </c>
-      <c r="I36" s="13"/>
+      <c r="I36" s="18"/>
     </row>
     <row r="37" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
@@ -1441,15 +1441,15 @@
       <c r="D37" s="8"/>
       <c r="E37" s="1"/>
       <c r="F37" s="9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H37" s="3">
         <v>0</v>
       </c>
-      <c r="I37" s="13"/>
+      <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
@@ -1458,36 +1458,36 @@
       <c r="D38" s="8"/>
       <c r="E38" s="1"/>
       <c r="F38" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H38" s="3">
         <v>0</v>
       </c>
-      <c r="I38" s="13"/>
+      <c r="I38" s="18"/>
     </row>
     <row r="39" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H39" s="3">
         <v>0</v>
       </c>
-      <c r="I39" s="13"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
@@ -1496,15 +1496,15 @@
       <c r="D40" s="8"/>
       <c r="E40" s="1"/>
       <c r="F40" s="9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H40" s="3">
         <v>0</v>
       </c>
-      <c r="I40" s="13"/>
+      <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="5"/>
@@ -1513,15 +1513,15 @@
       <c r="D41" s="8"/>
       <c r="E41" s="1"/>
       <c r="F41" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H41" s="3">
         <v>0</v>
       </c>
-      <c r="I41" s="14"/>
+      <c r="I41" s="19"/>
     </row>
     <row r="42" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
@@ -1535,7 +1535,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H42" s="3">
         <v>0</v>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H43" s="3">
         <v>0</v>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H44" s="3">
         <v>0</v>
@@ -1587,13 +1587,13 @@
         <v>6</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H45" s="3">
         <v>0</v>
@@ -1609,7 +1609,7 @@
         <v>14</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H46" s="3">
         <v>0</v>
@@ -1622,10 +1622,10 @@
       <c r="D47" s="8"/>
       <c r="E47" s="1"/>
       <c r="F47" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H47" s="3">
         <v>0</v>
@@ -1636,16 +1636,16 @@
       <c r="B48" s="6"/>
       <c r="C48" s="7"/>
       <c r="D48" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H48" s="3">
         <v>0</v>
@@ -1658,10 +1658,10 @@
       <c r="D49" s="8"/>
       <c r="E49" s="1"/>
       <c r="F49" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H49" s="3">
         <v>0</v>
@@ -1672,16 +1672,16 @@
       <c r="B50" s="6"/>
       <c r="C50" s="7"/>
       <c r="D50" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H50" s="3">
         <v>0</v>
@@ -1694,10 +1694,10 @@
       <c r="D51" s="8"/>
       <c r="E51" s="1"/>
       <c r="F51" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
@@ -1708,16 +1708,16 @@
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>
       <c r="D52" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H52" s="3">
         <v>0</v>
@@ -1730,10 +1730,10 @@
       <c r="D53" s="8"/>
       <c r="E53" s="1"/>
       <c r="F53" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H53" s="3">
         <v>0</v>
@@ -1752,10 +1752,10 @@
         <v>7</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H54" s="3">
         <v>0</v>
@@ -1771,7 +1771,7 @@
         <v>13</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H55" s="3">
         <v>0</v>
@@ -1787,7 +1787,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H56" s="3">
         <v>0</v>
@@ -1800,10 +1800,10 @@
       <c r="D57" s="8"/>
       <c r="E57" s="1"/>
       <c r="F57" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H57" s="3">
         <v>0</v>
@@ -1814,16 +1814,16 @@
       <c r="B58" s="6"/>
       <c r="C58" s="7"/>
       <c r="D58" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H58" s="3">
         <v>0</v>
@@ -1836,10 +1836,10 @@
       <c r="D59" s="8"/>
       <c r="E59" s="1"/>
       <c r="F59" s="9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H59" s="3">
         <v>0</v>
@@ -1852,10 +1852,10 @@
       <c r="D60" s="8"/>
       <c r="E60" s="1"/>
       <c r="F60" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H60" s="3">
         <v>0</v>
@@ -1873,7 +1873,7 @@
       <c r="E61" s="8"/>
       <c r="F61" s="8"/>
       <c r="G61" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H61" s="3">
         <v>0</v>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H62" s="3">
         <v>0</v>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H63" s="3">
         <v>0</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>1</v>
@@ -1927,13 +1927,13 @@
         <v>6</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H64" s="3">
         <v>0</v>
@@ -1949,7 +1949,7 @@
         <v>14</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H65" s="3">
         <v>0</v>
@@ -1962,10 +1962,10 @@
       <c r="D66" s="8"/>
       <c r="E66" s="1"/>
       <c r="F66" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -1976,16 +1976,16 @@
       <c r="B67" s="6"/>
       <c r="C67" s="7"/>
       <c r="D67" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H67" s="3">
         <v>0</v>
@@ -1998,10 +1998,10 @@
       <c r="D68" s="8"/>
       <c r="E68" s="1"/>
       <c r="F68" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H68" s="3">
         <v>0</v>
@@ -2012,16 +2012,16 @@
       <c r="B69" s="6"/>
       <c r="C69" s="7"/>
       <c r="D69" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H69" s="3">
         <v>0</v>
@@ -2034,10 +2034,10 @@
       <c r="D70" s="8"/>
       <c r="E70" s="1"/>
       <c r="F70" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H70" s="3">
         <v>0</v>
@@ -2048,16 +2048,16 @@
       <c r="B71" s="6"/>
       <c r="C71" s="7"/>
       <c r="D71" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H71" s="3">
         <v>0</v>
@@ -2070,10 +2070,10 @@
       <c r="D72" s="8"/>
       <c r="E72" s="1"/>
       <c r="F72" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H72" s="3">
         <v>0</v>
@@ -2092,10 +2092,10 @@
         <v>7</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H73" s="3">
         <v>0</v>
@@ -2111,7 +2111,7 @@
         <v>13</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H74" s="3">
         <v>0</v>
@@ -2127,7 +2127,7 @@
         <v>14</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H75" s="3">
         <v>0</v>
@@ -2140,10 +2140,10 @@
       <c r="D76" s="8"/>
       <c r="E76" s="1"/>
       <c r="F76" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H76" s="3">
         <v>0</v>
@@ -2154,16 +2154,16 @@
       <c r="B77" s="6"/>
       <c r="C77" s="7"/>
       <c r="D77" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H77" s="3">
         <v>0</v>
@@ -2176,10 +2176,10 @@
       <c r="D78" s="8"/>
       <c r="E78" s="1"/>
       <c r="F78" s="9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H78" s="3">
         <v>0</v>
@@ -2192,10 +2192,10 @@
       <c r="D79" s="8"/>
       <c r="E79" s="1"/>
       <c r="F79" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H79" s="3">
         <v>0</v>
@@ -2213,7 +2213,7 @@
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
       <c r="G80" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H80" s="3">
         <v>0</v>
@@ -2231,7 +2231,7 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H81" s="3">
         <v>0</v>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="F82" s="1"/>
       <c r="G82" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H82" s="3">
         <v>0</v>
@@ -2265,13 +2265,13 @@
         <v>6</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F83" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H83" s="3">
         <v>0</v>
@@ -2287,7 +2287,7 @@
         <v>14</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H84" s="3">
         <v>0</v>
@@ -2300,10 +2300,10 @@
       <c r="D85" s="8"/>
       <c r="E85" s="1"/>
       <c r="F85" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H85" s="3">
         <v>0</v>
@@ -2314,16 +2314,16 @@
       <c r="B86" s="6"/>
       <c r="C86" s="7"/>
       <c r="D86" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H86" s="3">
         <v>0</v>
@@ -2336,10 +2336,10 @@
       <c r="D87" s="8"/>
       <c r="E87" s="1"/>
       <c r="F87" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G87" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H87" s="3">
         <v>0</v>
@@ -2350,16 +2350,16 @@
       <c r="B88" s="6"/>
       <c r="C88" s="7"/>
       <c r="D88" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H88" s="3">
         <v>0</v>
@@ -2372,10 +2372,10 @@
       <c r="D89" s="8"/>
       <c r="E89" s="1"/>
       <c r="F89" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H89" s="3">
         <v>0</v>
@@ -2386,16 +2386,16 @@
       <c r="B90" s="6"/>
       <c r="C90" s="7"/>
       <c r="D90" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G90" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H90" s="3">
         <v>0</v>
@@ -2408,10 +2408,10 @@
       <c r="D91" s="8"/>
       <c r="E91" s="1"/>
       <c r="F91" s="9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H91" s="3">
         <v>0</v>
@@ -2430,10 +2430,10 @@
         <v>7</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H92" s="3">
         <v>0</v>
@@ -2449,7 +2449,7 @@
         <v>13</v>
       </c>
       <c r="G93" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H93" s="3">
         <v>0</v>
@@ -2465,7 +2465,7 @@
         <v>14</v>
       </c>
       <c r="G94" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H94" s="3">
         <v>0</v>
@@ -2478,10 +2478,10 @@
       <c r="D95" s="8"/>
       <c r="E95" s="1"/>
       <c r="F95" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H95" s="3">
         <v>0</v>
@@ -2492,16 +2492,16 @@
       <c r="B96" s="6"/>
       <c r="C96" s="7"/>
       <c r="D96" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H96" s="3">
         <v>0</v>
@@ -2514,10 +2514,10 @@
       <c r="D97" s="8"/>
       <c r="E97" s="1"/>
       <c r="F97" s="9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H97" s="3">
         <v>0</v>
@@ -2530,10 +2530,10 @@
       <c r="D98" s="8"/>
       <c r="E98" s="1"/>
       <c r="F98" s="9" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H98" s="3">
         <v>0</v>
@@ -2551,7 +2551,7 @@
       <c r="E99" s="8"/>
       <c r="F99" s="8"/>
       <c r="G99" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H99" s="3">
         <v>0</v>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H100" s="3">
         <v>0</v>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H101" s="3">
         <v>0</v>
@@ -2593,12 +2593,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I33:I41"/>
     <mergeCell ref="I2:I10"/>
     <mergeCell ref="J2:J5"/>
     <mergeCell ref="I11:I16"/>
     <mergeCell ref="I17:I22"/>
     <mergeCell ref="I23:I28"/>
-    <mergeCell ref="I33:I41"/>
   </mergeCells>
   <conditionalFormatting sqref="H2:H101">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
Changed structure -> more batch-size experiments
</commit_message>
<xml_diff>
--- a/Pytorch/Results/Structure.xlsx
+++ b/Pytorch/Results/Structure.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="49">
   <si>
     <t>CIFAR10</t>
   </si>
@@ -723,11 +723,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K101"/>
+  <dimension ref="A1:K104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,7 +767,7 @@
         <v>25</v>
       </c>
       <c r="H1" s="16">
-        <f>SUM(H2:H101)</f>
+        <f>SUM(H2:H104)</f>
         <v>4</v>
       </c>
       <c r="I1" s="12" t="s">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1085,7 +1085,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="I21" s="18"/>
     </row>
-    <row r="22" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
@@ -1174,7 +1174,7 @@
       </c>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
@@ -1197,7 +1197,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
@@ -1207,33 +1207,35 @@
         <v>45</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H24" s="3">
         <v>0</v>
       </c>
       <c r="I24" s="18"/>
-    </row>
-    <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J24" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H25" s="3">
         <v>0</v>
       </c>
       <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -1243,40 +1245,42 @@
         <v>45</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
       </c>
       <c r="I26" s="18"/>
-    </row>
-    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H27" s="3">
         <v>0</v>
       </c>
       <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J27" s="22"/>
+    </row>
+    <row r="28" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F28" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>30</v>
@@ -1284,22 +1288,16 @@
       <c r="H28" s="3">
         <v>0</v>
       </c>
-      <c r="I28" s="19"/>
-    </row>
-    <row r="29" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="1"/>
       <c r="F29" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>30</v>
@@ -1307,15 +1305,18 @@
       <c r="H29" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F30" s="9" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>30</v>
@@ -1323,15 +1324,16 @@
       <c r="H30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
       <c r="E31" s="1"/>
       <c r="F31" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>30</v>
@@ -1339,15 +1341,22 @@
       <c r="H31" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I31" s="19"/>
+    </row>
+    <row r="32" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="1"/>
+      <c r="C32" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F32" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>30</v>
@@ -1356,27 +1365,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="1"/>
       <c r="F33" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H33" s="3">
         <v>0</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
@@ -1386,7 +1388,7 @@
       <c r="D34" s="8"/>
       <c r="E34" s="1"/>
       <c r="F34" s="9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>30</v>
@@ -1394,16 +1396,15 @@
       <c r="H34" s="3">
         <v>0</v>
       </c>
-      <c r="I34" s="18"/>
-    </row>
-    <row r="35" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="5"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="8"/>
       <c r="E35" s="1"/>
       <c r="F35" s="9" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>30</v>
@@ -1411,14 +1412,13 @@
       <c r="H35" s="3">
         <v>0</v>
       </c>
-      <c r="I35" s="18"/>
-    </row>
-    <row r="36" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:9" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>7</v>
@@ -1432,7 +1432,9 @@
       <c r="H36" s="3">
         <v>0</v>
       </c>
-      <c r="I36" s="18"/>
+      <c r="I36" s="17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="37" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
@@ -1473,7 +1475,7 @@
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>7</v>
@@ -1506,7 +1508,7 @@
       </c>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -1521,77 +1523,74 @@
       <c r="H41" s="3">
         <v>0</v>
       </c>
-      <c r="I41" s="19"/>
+      <c r="I41" s="18"/>
     </row>
     <row r="42" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="C42" s="7"/>
       <c r="D42" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+        <v>33</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="G42" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H42" s="3">
         <v>0</v>
       </c>
+      <c r="I42" s="18"/>
     </row>
     <row r="43" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
-      <c r="D43" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F43" s="1"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="G43" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H43" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I43" s="18"/>
+    </row>
+    <row r="44" spans="1:9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
       <c r="D44" s="8"/>
-      <c r="E44" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="G44" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H44" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I44" s="19"/>
+    </row>
+    <row r="45" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
-      <c r="B45" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="B45" s="6"/>
       <c r="C45" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
       <c r="G45" s="4" t="s">
         <v>30</v>
       </c>
@@ -1599,15 +1598,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="D46" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="1"/>
       <c r="G46" s="4" t="s">
         <v>30</v>
       </c>
@@ -1615,15 +1616,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
       <c r="D47" s="8"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="E47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="1"/>
       <c r="G47" s="4" t="s">
         <v>30</v>
       </c>
@@ -1633,16 +1634,20 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="7"/>
+      <c r="B48" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D48" s="8" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>30</v>
@@ -1658,7 +1663,7 @@
       <c r="D49" s="8"/>
       <c r="E49" s="1"/>
       <c r="F49" s="9" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>30</v>
@@ -1671,14 +1676,10 @@
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="C50" s="7"/>
-      <c r="D50" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D50" s="8"/>
+      <c r="E50" s="1"/>
       <c r="F50" s="9" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>30</v>
@@ -1691,10 +1692,14 @@
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="1"/>
+      <c r="D51" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F51" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>30</v>
@@ -1707,14 +1712,10 @@
       <c r="A52" s="5"/>
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>
-      <c r="D52" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="1"/>
       <c r="F52" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>30</v>
@@ -1727,10 +1728,14 @@
       <c r="A53" s="5"/>
       <c r="B53" s="6"/>
       <c r="C53" s="7"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="1"/>
+      <c r="D53" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F53" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>30</v>
@@ -1742,17 +1747,11 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="1"/>
       <c r="F54" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>30</v>
@@ -1765,10 +1764,14 @@
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="C55" s="7"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="1"/>
+      <c r="D55" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F55" s="9" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>30</v>
@@ -1784,7 +1787,7 @@
       <c r="D56" s="8"/>
       <c r="E56" s="1"/>
       <c r="F56" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>30</v>
@@ -1796,11 +1799,17 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="1"/>
+      <c r="C57" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F57" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>30</v>
@@ -1813,14 +1822,10 @@
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
       <c r="C58" s="7"/>
-      <c r="D58" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D58" s="8"/>
+      <c r="E58" s="1"/>
       <c r="F58" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>30</v>
@@ -1836,7 +1841,7 @@
       <c r="D59" s="8"/>
       <c r="E59" s="1"/>
       <c r="F59" s="9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>30</v>
@@ -1852,7 +1857,7 @@
       <c r="D60" s="8"/>
       <c r="E60" s="1"/>
       <c r="F60" s="9" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>30</v>
@@ -1864,14 +1869,16 @@
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="C61" s="7"/>
       <c r="D61" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="G61" s="4" t="s">
         <v>30</v>
       </c>
@@ -1883,13 +1890,11 @@
       <c r="A62" s="5"/>
       <c r="B62" s="6"/>
       <c r="C62" s="7"/>
-      <c r="D62" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F62" s="1"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="G62" s="4" t="s">
         <v>30</v>
       </c>
@@ -1902,10 +1907,10 @@
       <c r="B63" s="6"/>
       <c r="C63" s="7"/>
       <c r="D63" s="8"/>
-      <c r="E63" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="G63" s="4" t="s">
         <v>30</v>
       </c>
@@ -1914,24 +1919,16 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="A64" s="5"/>
+      <c r="B64" s="6"/>
       <c r="C64" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
       <c r="G64" s="4" t="s">
         <v>30</v>
       </c>
@@ -1943,11 +1940,13 @@
       <c r="A65" s="5"/>
       <c r="B65" s="6"/>
       <c r="C65" s="7"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="D65" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F65" s="1"/>
       <c r="G65" s="4" t="s">
         <v>30</v>
       </c>
@@ -1960,10 +1959,10 @@
       <c r="B66" s="6"/>
       <c r="C66" s="7"/>
       <c r="D66" s="8"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="E66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F66" s="1"/>
       <c r="G66" s="4" t="s">
         <v>30</v>
       </c>
@@ -1972,17 +1971,23 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A67" s="5"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="7"/>
+      <c r="A67" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D67" s="8" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>30</v>
@@ -1998,7 +2003,7 @@
       <c r="D68" s="8"/>
       <c r="E68" s="1"/>
       <c r="F68" s="9" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>30</v>
@@ -2011,14 +2016,10 @@
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="7"/>
-      <c r="D69" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D69" s="8"/>
+      <c r="E69" s="1"/>
       <c r="F69" s="9" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>30</v>
@@ -2031,10 +2032,14 @@
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
       <c r="C70" s="7"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="1"/>
+      <c r="D70" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F70" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>30</v>
@@ -2047,14 +2052,10 @@
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
       <c r="C71" s="7"/>
-      <c r="D71" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D71" s="8"/>
+      <c r="E71" s="1"/>
       <c r="F71" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>30</v>
@@ -2067,10 +2068,14 @@
       <c r="A72" s="5"/>
       <c r="B72" s="6"/>
       <c r="C72" s="7"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="1"/>
+      <c r="D72" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F72" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>30</v>
@@ -2082,17 +2087,11 @@
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C73" s="7"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="1"/>
       <c r="F73" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>30</v>
@@ -2105,10 +2104,14 @@
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
       <c r="C74" s="7"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="1"/>
+      <c r="D74" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F74" s="9" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>30</v>
@@ -2124,7 +2127,7 @@
       <c r="D75" s="8"/>
       <c r="E75" s="1"/>
       <c r="F75" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>30</v>
@@ -2136,11 +2139,17 @@
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="5"/>
       <c r="B76" s="6"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="1"/>
+      <c r="C76" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F76" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>30</v>
@@ -2153,14 +2162,10 @@
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
       <c r="C77" s="7"/>
-      <c r="D77" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D77" s="8"/>
+      <c r="E77" s="1"/>
       <c r="F77" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>30</v>
@@ -2176,7 +2181,7 @@
       <c r="D78" s="8"/>
       <c r="E78" s="1"/>
       <c r="F78" s="9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>30</v>
@@ -2192,7 +2197,7 @@
       <c r="D79" s="8"/>
       <c r="E79" s="1"/>
       <c r="F79" s="9" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>30</v>
@@ -2204,14 +2209,16 @@
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="5"/>
       <c r="B80" s="6"/>
-      <c r="C80" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="C80" s="7"/>
       <c r="D80" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="G80" s="4" t="s">
         <v>30</v>
       </c>
@@ -2223,13 +2230,11 @@
       <c r="A81" s="5"/>
       <c r="B81" s="6"/>
       <c r="C81" s="7"/>
-      <c r="D81" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F81" s="1"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="G81" s="4" t="s">
         <v>30</v>
       </c>
@@ -2242,10 +2247,10 @@
       <c r="B82" s="6"/>
       <c r="C82" s="7"/>
       <c r="D82" s="8"/>
-      <c r="E82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="G82" s="4" t="s">
         <v>30</v>
       </c>
@@ -2255,21 +2260,15 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="5"/>
-      <c r="B83" s="6" t="s">
-        <v>2</v>
-      </c>
+      <c r="B83" s="6"/>
       <c r="C83" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E83" s="8"/>
+      <c r="F83" s="8"/>
       <c r="G83" s="4" t="s">
         <v>30</v>
       </c>
@@ -2281,11 +2280,13 @@
       <c r="A84" s="5"/>
       <c r="B84" s="6"/>
       <c r="C84" s="7"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="D84" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F84" s="1"/>
       <c r="G84" s="4" t="s">
         <v>30</v>
       </c>
@@ -2298,10 +2299,10 @@
       <c r="B85" s="6"/>
       <c r="C85" s="7"/>
       <c r="D85" s="8"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="E85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="1"/>
       <c r="G85" s="4" t="s">
         <v>30</v>
       </c>
@@ -2311,16 +2312,20 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="5"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="7"/>
+      <c r="B86" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D86" s="8" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>30</v>
@@ -2336,7 +2341,7 @@
       <c r="D87" s="8"/>
       <c r="E87" s="1"/>
       <c r="F87" s="9" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>30</v>
@@ -2349,14 +2354,10 @@
       <c r="A88" s="5"/>
       <c r="B88" s="6"/>
       <c r="C88" s="7"/>
-      <c r="D88" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D88" s="8"/>
+      <c r="E88" s="1"/>
       <c r="F88" s="9" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>30</v>
@@ -2369,10 +2370,14 @@
       <c r="A89" s="5"/>
       <c r="B89" s="6"/>
       <c r="C89" s="7"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="1"/>
+      <c r="D89" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F89" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>30</v>
@@ -2385,14 +2390,10 @@
       <c r="A90" s="5"/>
       <c r="B90" s="6"/>
       <c r="C90" s="7"/>
-      <c r="D90" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="D90" s="8"/>
+      <c r="E90" s="1"/>
       <c r="F90" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>30</v>
@@ -2405,10 +2406,14 @@
       <c r="A91" s="5"/>
       <c r="B91" s="6"/>
       <c r="C91" s="7"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="1"/>
+      <c r="D91" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F91" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>30</v>
@@ -2420,17 +2425,11 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="5"/>
       <c r="B92" s="6"/>
-      <c r="C92" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="C92" s="7"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="1"/>
       <c r="F92" s="9" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>30</v>
@@ -2443,10 +2442,14 @@
       <c r="A93" s="5"/>
       <c r="B93" s="6"/>
       <c r="C93" s="7"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="1"/>
+      <c r="D93" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F93" s="9" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>30</v>
@@ -2462,7 +2465,7 @@
       <c r="D94" s="8"/>
       <c r="E94" s="1"/>
       <c r="F94" s="9" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="G94" s="4" t="s">
         <v>30</v>
@@ -2474,11 +2477,17 @@
     <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="5"/>
       <c r="B95" s="6"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="1"/>
+      <c r="C95" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F95" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G95" s="4" t="s">
         <v>30</v>
@@ -2491,14 +2500,10 @@
       <c r="A96" s="5"/>
       <c r="B96" s="6"/>
       <c r="C96" s="7"/>
-      <c r="D96" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D96" s="8"/>
+      <c r="E96" s="1"/>
       <c r="F96" s="9" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>30</v>
@@ -2514,7 +2519,7 @@
       <c r="D97" s="8"/>
       <c r="E97" s="1"/>
       <c r="F97" s="9" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>30</v>
@@ -2530,7 +2535,7 @@
       <c r="D98" s="8"/>
       <c r="E98" s="1"/>
       <c r="F98" s="9" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>30</v>
@@ -2542,14 +2547,16 @@
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
-      <c r="C99" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="C99" s="7"/>
       <c r="D99" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="G99" s="4" t="s">
         <v>30</v>
       </c>
@@ -2561,13 +2568,11 @@
       <c r="A100" s="5"/>
       <c r="B100" s="6"/>
       <c r="C100" s="7"/>
-      <c r="D100" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F100" s="1"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="G100" s="4" t="s">
         <v>30</v>
       </c>
@@ -2580,27 +2585,80 @@
       <c r="B101" s="6"/>
       <c r="C101" s="7"/>
       <c r="D101" s="8"/>
-      <c r="E101" s="1" t="s">
+      <c r="E101" s="1"/>
+      <c r="F101" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G101" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H101" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A102" s="5"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" s="8"/>
+      <c r="F102" s="8"/>
+      <c r="G102" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H102" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A103" s="5"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F103" s="1"/>
+      <c r="G103" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H103" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A104" s="5"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F101" s="1"/>
-      <c r="G101" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H101" s="3">
+      <c r="F104" s="1"/>
+      <c r="G104" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H104" s="3">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="I33:I41"/>
+  <mergeCells count="7">
+    <mergeCell ref="I36:I44"/>
     <mergeCell ref="I2:I10"/>
     <mergeCell ref="J2:J5"/>
     <mergeCell ref="I11:I16"/>
     <mergeCell ref="I17:I22"/>
-    <mergeCell ref="I23:I28"/>
+    <mergeCell ref="I23:I31"/>
+    <mergeCell ref="J24:J27"/>
   </mergeCells>
-  <conditionalFormatting sqref="H2:H101">
+  <conditionalFormatting sqref="H2:H104">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Batch size results generated
</commit_message>
<xml_diff>
--- a/Pytorch/Results/Structure.xlsx
+++ b/Pytorch/Results/Structure.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Folder Structure" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="41">
   <si>
     <t>CIFAR10</t>
   </si>
@@ -137,6 +136,9 @@
   </si>
   <si>
     <t>lr=best</t>
+  </si>
+  <si>
+    <t>5-cycle</t>
   </si>
 </sst>
 </file>
@@ -708,11 +710,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -753,8 +755,8 @@
         <v>22</v>
       </c>
       <c r="H1" s="16">
-        <f>SUM(H3:H52)</f>
-        <v>8</v>
+        <f>SUM(H3:H63)</f>
+        <v>20</v>
       </c>
       <c r="J1" s="16"/>
       <c r="K1" s="15" t="s">
@@ -1133,7 +1135,7 @@
         <v>23</v>
       </c>
       <c r="H21" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="24" t="s">
         <v>31</v>
@@ -1153,7 +1155,7 @@
         <v>24</v>
       </c>
       <c r="H22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="25"/>
       <c r="J22" s="3"/>
@@ -1171,7 +1173,7 @@
         <v>25</v>
       </c>
       <c r="H23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="25"/>
       <c r="J23" s="3"/>
@@ -1189,7 +1191,7 @@
         <v>26</v>
       </c>
       <c r="H24" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="26"/>
       <c r="J24" s="3"/>
@@ -1232,7 +1234,7 @@
       </c>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -1258,77 +1260,73 @@
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H28" s="3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I28" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H29" s="3">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I29" s="25"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H30" s="3">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I30" s="25"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="8"/>
-      <c r="E31" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H31" s="3">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I31" s="26"/>
       <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
@@ -1337,7 +1335,7 @@
       <c r="C32" s="7"/>
       <c r="D32" s="8"/>
       <c r="E32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>39</v>
@@ -1350,20 +1348,16 @@
       </c>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
       <c r="E33" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>27</v>
@@ -1373,14 +1367,18 @@
       </c>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="1"/>
+      <c r="D34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F34" s="9" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>27</v>
@@ -1397,81 +1395,83 @@
       <c r="D35" s="8"/>
       <c r="E35" s="1"/>
       <c r="F35" s="9" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H35" s="3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I35" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="8"/>
       <c r="E36" s="1"/>
       <c r="F36" s="9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H36" s="3">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I36" s="25"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="8"/>
       <c r="E37" s="1"/>
       <c r="F37" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H37" s="3">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I37" s="25"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="5"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="1"/>
       <c r="F38" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H38" s="3">
-        <v>0</v>
-      </c>
-      <c r="J38" s="24" t="s">
-        <v>38</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I38" s="26"/>
+      <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="8"/>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="F39" s="9" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>27</v>
@@ -1479,16 +1479,18 @@
       <c r="H39" s="3">
         <v>0</v>
       </c>
-      <c r="J39" s="25"/>
+      <c r="J39" s="3"/>
     </row>
     <row r="40" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F40" s="9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>27</v>
@@ -1496,16 +1498,20 @@
       <c r="H40" s="3">
         <v>0</v>
       </c>
-      <c r="J40" s="25"/>
-    </row>
-    <row r="41" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="1"/>
+      <c r="D41" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F41" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>27</v>
@@ -1513,7 +1519,7 @@
       <c r="H41" s="3">
         <v>0</v>
       </c>
-      <c r="J41" s="26"/>
+      <c r="J41" s="3"/>
     </row>
     <row r="42" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
@@ -1553,18 +1559,20 @@
       </c>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D44" s="8" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>27</v>
@@ -1579,11 +1587,9 @@
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
       <c r="D45" s="8"/>
-      <c r="E45" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E45" s="1"/>
       <c r="F45" s="9" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>27</v>
@@ -1598,11 +1604,9 @@
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
       <c r="D46" s="8"/>
-      <c r="E46" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E46" s="1"/>
       <c r="F46" s="9" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>27</v>
@@ -1616,14 +1620,10 @@
       <c r="A47" s="5"/>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
-      <c r="D47" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="1"/>
       <c r="F47" s="9" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>27</v>
@@ -1633,16 +1633,14 @@
       </c>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
       <c r="C48" s="7"/>
       <c r="D48" s="8"/>
-      <c r="E48" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="E48" s="1"/>
       <c r="F48" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>27</v>
@@ -1652,16 +1650,18 @@
       </c>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="6"/>
       <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
+      <c r="D49" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="E49" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>27</v>
@@ -1669,73 +1669,284 @@
       <c r="H49" s="3">
         <v>0</v>
       </c>
-      <c r="J49" s="3"/>
+      <c r="J49" s="24" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="50" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="G50" s="4" t="s">
         <v>27</v>
       </c>
       <c r="H50" s="3">
         <v>0</v>
       </c>
-      <c r="J50" s="3"/>
+      <c r="J50" s="25"/>
     </row>
     <row r="51" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7"/>
-      <c r="D51" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" s="1"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="G51" s="4" t="s">
         <v>27</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
       </c>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="J51" s="25"/>
+    </row>
+    <row r="52" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="5"/>
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>
       <c r="D52" s="8"/>
-      <c r="E52" s="1" t="s">
+      <c r="E52" s="1"/>
+      <c r="F52" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="26"/>
+    </row>
+    <row r="53" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="5"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="5"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="5"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="5"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="5"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="5"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="5"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="5"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="5"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="5"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H52" s="3">
-        <v>0</v>
-      </c>
-      <c r="J52" s="3"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="J63" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="I7:I10"/>
     <mergeCell ref="I21:I24"/>
     <mergeCell ref="J17:J20"/>
-    <mergeCell ref="J38:J41"/>
+    <mergeCell ref="J49:J52"/>
     <mergeCell ref="I3:I6"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="I35:I38"/>
   </mergeCells>
-  <conditionalFormatting sqref="J22:J32 J2:J16 J47 J50:J52 H2:H52">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="J22:J27 J58 J2:J16 J61:J63 J32:J34 J39:J40 H2:H63">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1744,7 +1955,37 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J48:J49">
+  <conditionalFormatting sqref="J59:J60">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J53:J57">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J21">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J29:J31">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1754,7 +1995,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J42:J46">
+  <conditionalFormatting sqref="J28">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36:J38">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1764,8 +2015,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J21">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="J35">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41:J43">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
Defined more test cases for AdaSecant
</commit_message>
<xml_diff>
--- a/Pytorch/Results/Structure.xlsx
+++ b/Pytorch/Results/Structure.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="47">
   <si>
     <t>CIFAR10</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>combinations</t>
-  </si>
-  <si>
     <t>lr=0.01</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
   </si>
   <si>
     <t>Optimizer</t>
-  </si>
-  <si>
-    <t>Cycle</t>
-  </si>
-  <si>
-    <t>Decay</t>
   </si>
   <si>
     <t>LR</t>
@@ -136,6 +127,36 @@
   </si>
   <si>
     <t>lr=0.01-3</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>g_norm</t>
+  </si>
+  <si>
+    <t>Cycle / g</t>
+  </si>
+  <si>
+    <t>Decay / combinations</t>
+  </si>
+  <si>
+    <t>batch-size=129</t>
+  </si>
+  <si>
+    <t>batch-size=130</t>
+  </si>
+  <si>
+    <t>batch-size=131</t>
+  </si>
+  <si>
+    <t>batch-size=132</t>
+  </si>
+  <si>
+    <t>batch-size=133</t>
+  </si>
+  <si>
+    <t>batch-size=134</t>
   </si>
 </sst>
 </file>
@@ -733,11 +754,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -757,33 +778,33 @@
   <sheetData>
     <row r="1" spans="1:11" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" s="16">
-        <f>SUM(H2:H68)</f>
+        <f>SUM(H2:H69)</f>
         <v>33</v>
       </c>
       <c r="J1" s="16"/>
       <c r="K1" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -803,10 +824,10 @@
         <v>6</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H2" s="3">
         <v>1</v>
@@ -822,10 +843,10 @@
       <c r="D3" s="8"/>
       <c r="E3" s="1"/>
       <c r="F3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H3" s="3">
         <v>1</v>
@@ -841,16 +862,16 @@
       <c r="D4" s="8"/>
       <c r="E4" s="1"/>
       <c r="F4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H4" s="3">
         <v>1</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J4" s="3"/>
     </row>
@@ -861,10 +882,10 @@
       <c r="D5" s="8"/>
       <c r="E5" s="1"/>
       <c r="F5" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H5" s="3">
         <v>1</v>
@@ -879,10 +900,10 @@
       <c r="D6" s="8"/>
       <c r="E6" s="1"/>
       <c r="F6" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H6" s="3">
         <v>1</v>
@@ -897,10 +918,10 @@
       <c r="D7" s="8"/>
       <c r="E7" s="1"/>
       <c r="F7" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H7" s="3">
         <v>1</v>
@@ -915,16 +936,16 @@
       <c r="D8" s="8"/>
       <c r="E8" s="1"/>
       <c r="F8" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H8" s="3">
         <v>1</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J8" s="3"/>
     </row>
@@ -935,10 +956,10 @@
       <c r="D9" s="8"/>
       <c r="E9" s="1"/>
       <c r="F9" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3">
         <v>1</v>
@@ -953,10 +974,10 @@
       <c r="D10" s="8"/>
       <c r="E10" s="1"/>
       <c r="F10" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
@@ -971,10 +992,10 @@
       <c r="D11" s="8"/>
       <c r="E11" s="1"/>
       <c r="F11" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H11" s="3">
         <v>1</v>
@@ -989,10 +1010,10 @@
       <c r="D12" s="8"/>
       <c r="E12" s="1"/>
       <c r="F12" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H12" s="3">
         <v>1</v>
@@ -1006,10 +1027,10 @@
       <c r="D13" s="8"/>
       <c r="E13" s="1"/>
       <c r="F13" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
@@ -1025,10 +1046,10 @@
         <v>7</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H14" s="3">
         <v>0</v>
@@ -1042,10 +1063,10 @@
       <c r="D15" s="8"/>
       <c r="E15" s="1"/>
       <c r="F15" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H15" s="3">
         <v>0</v>
@@ -1059,10 +1080,10 @@
       <c r="D16" s="8"/>
       <c r="E16" s="1"/>
       <c r="F16" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H16" s="3">
         <v>0</v>
@@ -1076,10 +1097,10 @@
       <c r="D17" s="8"/>
       <c r="E17" s="1"/>
       <c r="F17" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H17" s="3">
         <v>0</v>
@@ -1093,10 +1114,10 @@
       <c r="D18" s="8"/>
       <c r="E18" s="1"/>
       <c r="F18" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H18" s="3">
         <v>0</v>
@@ -1108,23 +1129,23 @@
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H19" s="3">
         <v>1</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1134,10 +1155,10 @@
       <c r="D20" s="8"/>
       <c r="E20" s="1"/>
       <c r="F20" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H20" s="3">
         <v>1</v>
@@ -1152,10 +1173,10 @@
       <c r="D21" s="8"/>
       <c r="E21" s="1"/>
       <c r="F21" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H21" s="3">
         <v>1</v>
@@ -1170,16 +1191,16 @@
       <c r="D22" s="8"/>
       <c r="E22" s="1"/>
       <c r="F22" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H22" s="3">
         <v>1</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J22" s="28"/>
     </row>
@@ -1190,10 +1211,10 @@
       <c r="D23" s="8"/>
       <c r="E23" s="1"/>
       <c r="F23" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H23" s="3">
         <v>1</v>
@@ -1208,10 +1229,10 @@
       <c r="D24" s="8"/>
       <c r="E24" s="1"/>
       <c r="F24" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H24" s="3">
         <v>1</v>
@@ -1226,10 +1247,10 @@
       <c r="D25" s="8"/>
       <c r="E25" s="1"/>
       <c r="F25" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H25" s="3">
         <v>1</v>
@@ -1246,10 +1267,10 @@
         <v>8</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H26" s="3">
         <v>0</v>
@@ -1265,10 +1286,10 @@
         <v>9</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H27" s="3">
         <v>0</v>
@@ -1280,23 +1301,23 @@
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H28" s="3">
         <v>1</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1306,10 +1327,10 @@
       <c r="D29" s="8"/>
       <c r="E29" s="1"/>
       <c r="F29" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H29" s="3">
         <v>1</v>
@@ -1324,10 +1345,10 @@
       <c r="D30" s="8"/>
       <c r="E30" s="1"/>
       <c r="F30" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H30" s="3">
         <v>1</v>
@@ -1342,16 +1363,16 @@
       <c r="D31" s="8"/>
       <c r="E31" s="1"/>
       <c r="F31" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H31" s="3">
         <v>1</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J31" s="28"/>
     </row>
@@ -1362,10 +1383,10 @@
       <c r="D32" s="8"/>
       <c r="E32" s="1"/>
       <c r="F32" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H32" s="3">
         <v>1</v>
@@ -1380,10 +1401,10 @@
       <c r="D33" s="8"/>
       <c r="E33" s="1"/>
       <c r="F33" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H33" s="3">
         <v>1</v>
@@ -1398,10 +1419,10 @@
       <c r="D34" s="8"/>
       <c r="E34" s="1"/>
       <c r="F34" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H34" s="3">
         <v>1</v>
@@ -1418,10 +1439,10 @@
         <v>8</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H35" s="3">
         <v>0</v>
@@ -1437,10 +1458,10 @@
         <v>9</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H36" s="3">
         <v>0</v>
@@ -1452,23 +1473,23 @@
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H37" s="3">
         <v>1</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1478,10 +1499,10 @@
       <c r="D38" s="8"/>
       <c r="E38" s="1"/>
       <c r="F38" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H38" s="3">
         <v>1</v>
@@ -1496,10 +1517,10 @@
       <c r="D39" s="8"/>
       <c r="E39" s="1"/>
       <c r="F39" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H39" s="3">
         <v>1</v>
@@ -1514,16 +1535,16 @@
       <c r="D40" s="8"/>
       <c r="E40" s="1"/>
       <c r="F40" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H40" s="3">
         <v>1</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J40" s="28"/>
     </row>
@@ -1534,10 +1555,10 @@
       <c r="D41" s="8"/>
       <c r="E41" s="1"/>
       <c r="F41" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H41" s="3">
         <v>1</v>
@@ -1552,10 +1573,10 @@
       <c r="D42" s="8"/>
       <c r="E42" s="1"/>
       <c r="F42" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H42" s="3">
         <v>1</v>
@@ -1570,10 +1591,10 @@
       <c r="D43" s="8"/>
       <c r="E43" s="1"/>
       <c r="F43" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H43" s="3">
         <v>1</v>
@@ -1590,10 +1611,10 @@
         <v>8</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H44" s="3">
         <v>0</v>
@@ -1609,10 +1630,10 @@
         <v>9</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H45" s="3">
         <v>0</v>
@@ -1624,16 +1645,16 @@
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
       <c r="D46" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H46" s="3">
         <v>0</v>
@@ -1649,10 +1670,10 @@
         <v>8</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H47" s="3">
         <v>0</v>
@@ -1668,10 +1689,10 @@
         <v>9</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H48" s="3">
         <v>0</v>
@@ -1691,10 +1712,10 @@
         <v>6</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H49" s="3">
         <v>0</v>
@@ -1708,10 +1729,10 @@
       <c r="D50" s="8"/>
       <c r="E50" s="1"/>
       <c r="F50" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H50" s="3">
         <v>0</v>
@@ -1725,10 +1746,10 @@
       <c r="D51" s="8"/>
       <c r="E51" s="1"/>
       <c r="F51" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
@@ -1742,10 +1763,10 @@
       <c r="D52" s="8"/>
       <c r="E52" s="1"/>
       <c r="F52" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H52" s="3">
         <v>0</v>
@@ -1759,10 +1780,10 @@
       <c r="D53" s="8"/>
       <c r="E53" s="1"/>
       <c r="F53" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H53" s="3">
         <v>0</v>
@@ -1774,22 +1795,22 @@
       <c r="B54" s="6"/>
       <c r="C54" s="7"/>
       <c r="D54" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F54" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="J54" s="24" t="s">
         <v>31</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H54" s="3">
-        <v>0</v>
-      </c>
-      <c r="J54" s="24" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
@@ -1799,10 +1820,10 @@
       <c r="D55" s="8"/>
       <c r="E55" s="1"/>
       <c r="F55" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H55" s="3">
         <v>0</v>
@@ -1816,10 +1837,10 @@
       <c r="D56" s="8"/>
       <c r="E56" s="1"/>
       <c r="F56" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H56" s="3">
         <v>0</v>
@@ -1833,10 +1854,10 @@
       <c r="D57" s="8"/>
       <c r="E57" s="1"/>
       <c r="F57" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H57" s="3">
         <v>0</v>
@@ -1852,10 +1873,10 @@
         <v>8</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H58" s="3">
         <v>0</v>
@@ -1871,10 +1892,10 @@
         <v>9</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H59" s="3">
         <v>0</v>
@@ -1886,16 +1907,16 @@
       <c r="B60" s="6"/>
       <c r="C60" s="7"/>
       <c r="D60" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H60" s="3">
         <v>0</v>
@@ -1911,10 +1932,10 @@
         <v>8</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H61" s="3">
         <v>0</v>
@@ -1930,10 +1951,10 @@
         <v>9</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H62" s="3">
         <v>0</v>
@@ -1945,16 +1966,16 @@
       <c r="B63" s="6"/>
       <c r="C63" s="7"/>
       <c r="D63" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H63" s="3">
         <v>0</v>
@@ -1970,10 +1991,10 @@
         <v>8</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H64" s="3">
         <v>0</v>
@@ -1989,10 +2010,10 @@
         <v>9</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H65" s="3">
         <v>0</v>
@@ -2006,12 +2027,14 @@
         <v>4</v>
       </c>
       <c r="D66" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
+      <c r="F66" s="9"/>
       <c r="G66" s="4" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -2022,15 +2045,13 @@
       <c r="A67" s="5"/>
       <c r="B67" s="6"/>
       <c r="C67" s="7"/>
-      <c r="D67" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="D67" s="8"/>
       <c r="E67" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F67" s="1"/>
+      <c r="F67" s="9"/>
       <c r="G67" s="4" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="H67" s="3">
         <v>0</v>
@@ -2041,18 +2062,70 @@
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="C68" s="7"/>
-      <c r="D68" s="8"/>
+      <c r="D68" s="10"/>
       <c r="E68" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F68" s="1"/>
+      <c r="F68" s="9"/>
       <c r="G68" s="4" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="H68" s="3">
         <v>0</v>
       </c>
       <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="9"/>
+      <c r="G69" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="5"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F70" s="9"/>
+      <c r="G70" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H70" s="3">
+        <v>0</v>
+      </c>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A71" s="5"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F71" s="9"/>
+      <c r="G71" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2066,8 +2139,8 @@
     <mergeCell ref="J28:J34"/>
     <mergeCell ref="J19:J25"/>
   </mergeCells>
-  <conditionalFormatting sqref="J2:J18 J63 J66:J68 J26:J27 H35:H36 J35:J36 H46:H68 H2:H27">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="J2:J18 J63 J66:J70 J26:J27 H35:H36 J35:J36 H2:H27 H46:H71">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2077,7 +2150,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J64:J65">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2087,7 +2160,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J58:J62">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2097,6 +2170,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:J48">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28:H34">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2106,18 +2189,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28:H34">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H44:H45 J44:J45">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2127,7 +2200,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37:H43">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
Updated for new data
</commit_message>
<xml_diff>
--- a/Pytorch/Results/Structure.xlsx
+++ b/Pytorch/Results/Structure.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="46">
   <si>
     <t>CIFAR10</t>
   </si>
@@ -151,13 +151,16 @@
   </si>
   <si>
     <t>CIFAR100</t>
+  </si>
+  <si>
+    <t>best-cycle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,6 +177,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -356,10 +366,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -409,6 +420,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -431,7 +445,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,11 +749,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,13 +795,16 @@
       </c>
       <c r="H1" s="16">
         <f>SUM(H2:H48)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I1" s="12">
-        <f>COUNT(H2:H87)</f>
-        <v>86</v>
-      </c>
-      <c r="J1" s="16"/>
+        <f>COUNT(H2:H79)</f>
+        <v>78</v>
+      </c>
+      <c r="J1" s="21">
+        <f>H1/I1</f>
+        <v>8.9743589743589744E-2</v>
+      </c>
       <c r="K1" s="15" t="s">
         <v>21</v>
       </c>
@@ -852,9 +870,9 @@
         <v>16</v>
       </c>
       <c r="H4" s="3">
-        <v>0</v>
-      </c>
-      <c r="I4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="3"/>
@@ -874,7 +892,7 @@
       <c r="H5" s="3">
         <v>1</v>
       </c>
-      <c r="I5" s="22"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -890,9 +908,9 @@
         <v>18</v>
       </c>
       <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="23"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
@@ -908,9 +926,9 @@
         <v>16</v>
       </c>
       <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J7" s="3"/>
@@ -928,9 +946,9 @@
         <v>17</v>
       </c>
       <c r="H8" s="3">
-        <v>0</v>
-      </c>
-      <c r="I8" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="23"/>
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
@@ -946,9 +964,9 @@
         <v>18</v>
       </c>
       <c r="H9" s="3">
-        <v>0</v>
-      </c>
-      <c r="I9" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="23"/>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
@@ -1092,7 +1110,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="27" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1112,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="27"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="1:10" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
@@ -1130,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="27"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
@@ -1147,10 +1165,10 @@
       <c r="H20" s="3">
         <v>0</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="27"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
@@ -1165,10 +1183,10 @@
         <v>17</v>
       </c>
       <c r="H21" s="3">
-        <v>0</v>
-      </c>
-      <c r="I21" s="24"/>
-      <c r="J21" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="25"/>
+      <c r="J21" s="28"/>
     </row>
     <row r="22" spans="1:10" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="5"/>
@@ -1185,8 +1203,8 @@
       <c r="H22" s="3">
         <v>0</v>
       </c>
-      <c r="I22" s="24"/>
-      <c r="J22" s="27"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="28"/>
     </row>
     <row r="23" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
@@ -1208,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="2"/>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="27" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1228,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="2"/>
-      <c r="J24" s="27"/>
+      <c r="J24" s="28"/>
     </row>
     <row r="25" spans="1:10" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5"/>
@@ -1246,7 +1264,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="27"/>
+      <c r="J25" s="28"/>
     </row>
     <row r="26" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
@@ -1263,10 +1281,10 @@
       <c r="H26" s="3">
         <v>0</v>
       </c>
-      <c r="I26" s="23" t="s">
+      <c r="I26" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="27"/>
+      <c r="J26" s="28"/>
     </row>
     <row r="27" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
@@ -1283,8 +1301,8 @@
       <c r="H27" s="3">
         <v>0</v>
       </c>
-      <c r="I27" s="24"/>
-      <c r="J27" s="27"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="5"/>
@@ -1301,8 +1319,8 @@
       <c r="H28" s="3">
         <v>0</v>
       </c>
-      <c r="I28" s="24"/>
-      <c r="J28" s="27"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
@@ -1324,7 +1342,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="2"/>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="27" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1344,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="2"/>
-      <c r="J30" s="27"/>
+      <c r="J30" s="28"/>
     </row>
     <row r="31" spans="1:10" customFormat="1" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="5"/>
@@ -1362,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="2"/>
-      <c r="J31" s="27"/>
+      <c r="J31" s="28"/>
     </row>
     <row r="32" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
@@ -1379,10 +1397,10 @@
       <c r="H32" s="3">
         <v>0</v>
       </c>
-      <c r="I32" s="23" t="s">
+      <c r="I32" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="J32" s="27"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
@@ -1399,8 +1417,8 @@
       <c r="H33" s="3">
         <v>0</v>
       </c>
-      <c r="I33" s="24"/>
-      <c r="J33" s="27"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="28"/>
     </row>
     <row r="34" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
@@ -1417,8 +1435,8 @@
       <c r="H34" s="3">
         <v>0</v>
       </c>
-      <c r="I34" s="24"/>
-      <c r="J34" s="27"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="28"/>
     </row>
     <row r="35" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
@@ -1530,7 +1548,7 @@
       <c r="H40" s="3">
         <v>0</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="J40" s="24" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1549,7 +1567,7 @@
       <c r="H41" s="3">
         <v>0</v>
       </c>
-      <c r="J41" s="24"/>
+      <c r="J41" s="25"/>
     </row>
     <row r="42" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
@@ -1566,7 +1584,7 @@
       <c r="H42" s="3">
         <v>0</v>
       </c>
-      <c r="J42" s="24"/>
+      <c r="J42" s="25"/>
     </row>
     <row r="43" spans="1:10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="5"/>
@@ -1583,7 +1601,7 @@
       <c r="H43" s="3">
         <v>0</v>
       </c>
-      <c r="J43" s="25"/>
+      <c r="J43" s="26"/>
     </row>
     <row r="44" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
@@ -1800,7 +1818,7 @@
       <c r="B54" s="6"/>
       <c r="C54" s="7"/>
       <c r="D54" s="8" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>5</v>
@@ -1820,15 +1838,17 @@
     <row r="55" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
-      <c r="C55" s="7"/>
+      <c r="C55" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="D55" s="8" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>17</v>
@@ -1844,7 +1864,7 @@
       <c r="B56" s="6"/>
       <c r="C56" s="7"/>
       <c r="D56" s="8" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>5</v>
@@ -1861,11 +1881,11 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="6"/>
       <c r="C57" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>4</v>
@@ -1874,7 +1894,7 @@
         <v>5</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>17</v>
@@ -1882,21 +1902,22 @@
       <c r="H57" s="3">
         <v>0</v>
       </c>
-      <c r="I57" s="3"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="6"/>
-      <c r="C58" s="7"/>
+      <c r="C58" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D58" s="8" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>17</v>
@@ -1904,21 +1925,22 @@
       <c r="H58" s="3">
         <v>0</v>
       </c>
-      <c r="I58" s="3"/>
       <c r="J58" s="3"/>
     </row>
     <row r="59" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="7"/>
+      <c r="C59" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="D59" s="8" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>17</v>
@@ -1926,15 +1948,20 @@
       <c r="H59" s="3">
         <v>0</v>
       </c>
-      <c r="I59" s="3"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6"/>
-      <c r="C60" s="7"/>
+    <row r="60" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D60" s="8" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>5</v>
@@ -1948,19 +1975,17 @@
       <c r="H60" s="3">
         <v>0</v>
       </c>
+      <c r="I60" s="3"/>
       <c r="J60" s="3"/>
+      <c r="K60" s="19"/>
     </row>
     <row r="61" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="6"/>
-      <c r="C61" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="C61" s="7"/>
+      <c r="D61" s="8"/>
       <c r="E61" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>27</v>
@@ -1971,22 +1996,21 @@
       <c r="H61" s="3">
         <v>0</v>
       </c>
+      <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="C62" s="7"/>
       <c r="D62" s="8" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>17</v>
@@ -1994,22 +2018,21 @@
       <c r="H62" s="3">
         <v>0</v>
       </c>
+      <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="C63" s="7"/>
       <c r="D63" s="8" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>17</v>
@@ -2017,20 +2040,15 @@
       <c r="H63" s="3">
         <v>0</v>
       </c>
+      <c r="I63" s="3"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>2</v>
-      </c>
+    <row r="64" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="5"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="7"/>
       <c r="D64" s="8" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>5</v>
@@ -2046,15 +2064,18 @@
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
-      <c r="K64" s="19"/>
-    </row>
-    <row r="65" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="8"/>
+      <c r="C65" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E65" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>27</v>
@@ -2090,7 +2111,7 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="6"/>
       <c r="C67" s="7"/>
@@ -2112,7 +2133,7 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5"/>
       <c r="B68" s="6"/>
       <c r="C68" s="7"/>
@@ -2131,14 +2152,13 @@
       <c r="H68" s="3">
         <v>0</v>
       </c>
-      <c r="I68" s="3"/>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5"/>
       <c r="B69" s="6"/>
       <c r="C69" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>4</v>
@@ -2155,21 +2175,22 @@
       <c r="H69" s="3">
         <v>0</v>
       </c>
-      <c r="I69" s="3"/>
       <c r="J69" s="3"/>
     </row>
-    <row r="70" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5"/>
       <c r="B70" s="6"/>
-      <c r="C70" s="7"/>
+      <c r="C70" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D70" s="8" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>17</v>
@@ -2177,21 +2198,22 @@
       <c r="H70" s="3">
         <v>0</v>
       </c>
-      <c r="I70" s="3"/>
       <c r="J70" s="3"/>
     </row>
     <row r="71" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="7"/>
+      <c r="C71" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="D71" s="8" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>17</v>
@@ -2199,15 +2221,20 @@
       <c r="H71" s="3">
         <v>0</v>
       </c>
-      <c r="I71" s="3"/>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="5"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="7"/>
+    <row r="72" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D72" s="8" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>5</v>
@@ -2221,19 +2248,17 @@
       <c r="H72" s="3">
         <v>0</v>
       </c>
+      <c r="I72" s="3"/>
       <c r="J72" s="3"/>
+      <c r="K72" s="19"/>
     </row>
     <row r="73" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5"/>
       <c r="B73" s="6"/>
-      <c r="C73" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="C73" s="7"/>
+      <c r="D73" s="8"/>
       <c r="E73" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>27</v>
@@ -2244,22 +2269,21 @@
       <c r="H73" s="3">
         <v>0</v>
       </c>
+      <c r="I73" s="3"/>
       <c r="J73" s="3"/>
     </row>
-    <row r="74" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="6"/>
-      <c r="C74" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="C74" s="7"/>
       <c r="D74" s="8" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>17</v>
@@ -2267,22 +2291,23 @@
       <c r="H74" s="3">
         <v>0</v>
       </c>
+      <c r="I74" s="3"/>
       <c r="J74" s="3"/>
     </row>
-    <row r="75" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5"/>
       <c r="B75" s="6"/>
       <c r="C75" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>17</v>
@@ -2290,20 +2315,15 @@
       <c r="H75" s="3">
         <v>0</v>
       </c>
+      <c r="I75" s="3"/>
       <c r="J75" s="3"/>
     </row>
-    <row r="76" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>2</v>
-      </c>
+    <row r="76" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="5"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="7"/>
       <c r="D76" s="8" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>5</v>
@@ -2319,15 +2339,18 @@
       </c>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
-      <c r="K76" s="19"/>
     </row>
     <row r="77" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="6"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="8"/>
+      <c r="C77" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E77" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>27</v>
@@ -2338,21 +2361,22 @@
       <c r="H77" s="3">
         <v>0</v>
       </c>
-      <c r="I77" s="3"/>
       <c r="J77" s="3"/>
     </row>
-    <row r="78" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="5"/>
       <c r="B78" s="6"/>
-      <c r="C78" s="7"/>
+      <c r="C78" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D78" s="8" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>17</v>
@@ -2360,21 +2384,22 @@
       <c r="H78" s="3">
         <v>0</v>
       </c>
-      <c r="I78" s="3"/>
       <c r="J78" s="3"/>
     </row>
-    <row r="79" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="5"/>
       <c r="B79" s="6"/>
-      <c r="C79" s="7"/>
+      <c r="C79" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="D79" s="8" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>17</v>
@@ -2382,188 +2407,7 @@
       <c r="H79" s="3">
         <v>0</v>
       </c>
-      <c r="I79" s="3"/>
       <c r="J79" s="3"/>
-    </row>
-    <row r="80" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="5"/>
-      <c r="B80" s="6"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H80" s="3">
-        <v>0</v>
-      </c>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-    </row>
-    <row r="81" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="5"/>
-      <c r="B81" s="6"/>
-      <c r="C81" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H81" s="3">
-        <v>0</v>
-      </c>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-    </row>
-    <row r="82" spans="1:10" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="5"/>
-      <c r="B82" s="6"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H82" s="3">
-        <v>0</v>
-      </c>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-    </row>
-    <row r="83" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="5"/>
-      <c r="B83" s="6"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H83" s="3">
-        <v>0</v>
-      </c>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-    </row>
-    <row r="84" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="5"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G84" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H84" s="3">
-        <v>0</v>
-      </c>
-      <c r="J84" s="3"/>
-    </row>
-    <row r="85" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="5"/>
-      <c r="B85" s="6"/>
-      <c r="C85" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G85" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H85" s="3">
-        <v>0</v>
-      </c>
-      <c r="J85" s="3"/>
-    </row>
-    <row r="86" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="5"/>
-      <c r="B86" s="6"/>
-      <c r="C86" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G86" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H86" s="3">
-        <v>0</v>
-      </c>
-      <c r="J86" s="3"/>
-    </row>
-    <row r="87" spans="1:10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="5"/>
-      <c r="B87" s="6"/>
-      <c r="C87" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H87" s="3">
-        <v>0</v>
-      </c>
-      <c r="J87" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2587,7 +2431,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J61">
+  <conditionalFormatting sqref="J57">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -2597,17 +2441,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51:J59">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J62:J63 J60">
+  <conditionalFormatting sqref="J58:J59">
     <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min"/>
@@ -2617,17 +2451,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J45:J49 J2:J16 H2:H87">
-    <cfRule type="colorScale" priority="88">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J73">
+  <conditionalFormatting sqref="J69">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -2637,7 +2461,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I64:J71">
+  <conditionalFormatting sqref="I60:J67">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2647,7 +2471,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J74:J75 J72">
+  <conditionalFormatting sqref="J70:J71 J68">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -2657,7 +2481,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J85">
+  <conditionalFormatting sqref="J77">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2667,8 +2491,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I76:J83">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="J78:J79">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2677,8 +2501,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J86:J87 J84">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="I51:J56">
+    <cfRule type="colorScale" priority="93">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I72:J76">
+    <cfRule type="colorScale" priority="100">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45:J49 J2:J16 H2:H79">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
Analyzed Adam, changed structure of experiments to allow for lower lr_max instead of larger base_lr. This is because Adam with high lr does not perform well. We hope to stay in a better range.
</commit_message>
<xml_diff>
--- a/Pytorch/Results/Structure.xlsx
+++ b/Pytorch/Results/Structure.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="50">
   <si>
     <t>CIFAR10</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>lr=0.0001</t>
+  </si>
+  <si>
+    <t>lr=0.0001-0.1</t>
+  </si>
+  <si>
+    <t>lr=0.0001-0.3</t>
+  </si>
+  <si>
+    <t>lr=0.0001-0.01</t>
+  </si>
+  <si>
+    <t>lr=0.0001-0.03</t>
   </si>
 </sst>
 </file>
@@ -749,8 +761,8 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -760,7 +772,7 @@
     <col min="3" max="3" width="9.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.1796875" style="3" customWidth="1"/>
     <col min="9" max="9" width="8.7265625" style="2"/>
@@ -1480,7 +1492,7 @@
         <v>5</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>17</v>
@@ -1499,7 +1511,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="1"/>
       <c r="F38" s="9" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>17</v>
@@ -1516,7 +1528,7 @@
       <c r="D39" s="8"/>
       <c r="E39" s="1"/>
       <c r="F39" s="9" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>17</v>
@@ -1533,7 +1545,7 @@
       <c r="D40" s="8"/>
       <c r="E40" s="1"/>
       <c r="F40" s="9" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Changed Plot style after feedback
</commit_message>
<xml_diff>
--- a/Pytorch/Results/Structure.xlsx
+++ b/Pytorch/Results/Structure.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="56">
   <si>
     <t>CIFAR10</t>
   </si>
@@ -150,9 +150,6 @@
     <t>CIFAR100</t>
   </si>
   <si>
-    <t>best-cycle</t>
-  </si>
-  <si>
     <t>lr=0.0001</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>SASSE</t>
+  </si>
+  <si>
+    <t>accidental run</t>
   </si>
 </sst>
 </file>
@@ -779,8 +779,8 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J58" sqref="J58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -822,7 +822,7 @@
       </c>
       <c r="H1" s="15">
         <f>SUM(H2:H63)</f>
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I1" s="11">
         <f>COUNT(H2:H63)</f>
@@ -830,7 +830,7 @@
       </c>
       <c r="J1" s="20">
         <f>H1/I1</f>
-        <v>0.75806451612903225</v>
+        <v>0.9838709677419355</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>21</v>
@@ -1026,7 +1026,7 @@
         <v>17</v>
       </c>
       <c r="H11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="3"/>
     </row>
@@ -1043,7 +1043,7 @@
         <v>17</v>
       </c>
       <c r="H12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="3"/>
     </row>
@@ -1362,7 +1362,7 @@
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>5</v>
@@ -1392,7 +1392,7 @@
         <v>5</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>17</v>
@@ -1515,7 +1515,7 @@
         <v>5</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>17</v>
@@ -1524,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="I37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J37" s="23" t="s">
         <v>26</v>
@@ -1537,7 +1537,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="1"/>
       <c r="F38" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>17</v>
@@ -1546,7 +1546,7 @@
         <v>1</v>
       </c>
       <c r="I38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J38" s="24"/>
     </row>
@@ -1557,16 +1557,16 @@
       <c r="D39" s="8"/>
       <c r="E39" s="1"/>
       <c r="F39" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
         <v>52</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" s="3">
-        <v>1</v>
-      </c>
-      <c r="I39" t="s">
-        <v>53</v>
       </c>
       <c r="J39" s="24"/>
     </row>
@@ -1577,7 +1577,7 @@
       <c r="D40" s="8"/>
       <c r="E40" s="1"/>
       <c r="F40" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>17</v>
@@ -1586,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="I40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J40" s="25"/>
     </row>
@@ -1597,7 +1597,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="1"/>
       <c r="F41" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>17</v>
@@ -1606,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="I41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J41" s="3"/>
     </row>
@@ -1617,7 +1617,7 @@
       <c r="D42" s="8"/>
       <c r="E42" s="1"/>
       <c r="F42" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>17</v>
@@ -1626,7 +1626,7 @@
         <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J42" s="3"/>
     </row>
@@ -1641,7 +1641,7 @@
         <v>5</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>17</v>
@@ -1662,13 +1662,13 @@
         <v>5</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H44" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="3"/>
     </row>
@@ -1691,7 +1691,7 @@
         <v>17</v>
       </c>
       <c r="H45" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J45" s="3"/>
     </row>
@@ -1778,7 +1778,7 @@
       <c r="A50" s="5"/>
       <c r="B50" s="6"/>
       <c r="C50" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>24</v>
@@ -1867,7 +1867,7 @@
         <v>17</v>
       </c>
       <c r="H53" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
@@ -1877,19 +1877,19 @@
       <c r="B54" s="6"/>
       <c r="C54" s="7"/>
       <c r="D54" s="8" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H54" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
@@ -1913,7 +1913,7 @@
         <v>17</v>
       </c>
       <c r="H55" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J55" s="3"/>
     </row>
@@ -1945,7 +1945,7 @@
         <v>43</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>2</v>
@@ -1963,47 +1963,42 @@
         <v>17</v>
       </c>
       <c r="H57" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="18"/>
     </row>
-    <row r="58" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>2</v>
-      </c>
+    <row r="58" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="5"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="7"/>
       <c r="D58" s="8" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H58" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="18"/>
     </row>
     <row r="59" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="7"/>
+      <c r="C59" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="D59" s="8" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>5</v>
@@ -2015,7 +2010,7 @@
         <v>17</v>
       </c>
       <c r="H59" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
@@ -2023,11 +2018,9 @@
     <row r="60" spans="1:11" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="C60" s="7"/>
       <c r="D60" s="8" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>5</v>
@@ -2039,7 +2032,7 @@
         <v>17</v>
       </c>
       <c r="H60" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
@@ -2049,7 +2042,7 @@
       <c r="B61" s="6"/>
       <c r="C61" s="7"/>
       <c r="D61" s="8" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>5</v>
@@ -2061,9 +2054,11 @@
         <v>17</v>
       </c>
       <c r="H61" s="3">
-        <v>0</v>
-      </c>
-      <c r="I61" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="J61" s="3"/>
     </row>
     <row r="62" spans="1:11" customFormat="1" x14ac:dyDescent="0.35">
@@ -2085,7 +2080,7 @@
         <v>17</v>
       </c>
       <c r="H62" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" s="3"/>
     </row>
@@ -2108,7 +2103,7 @@
         <v>17</v>
       </c>
       <c r="H63" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" s="3"/>
     </row>
@@ -2124,7 +2119,7 @@
     <mergeCell ref="J13:J18"/>
   </mergeCells>
   <conditionalFormatting sqref="J43">
-    <cfRule type="colorScale" priority="76">
+    <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2134,7 +2129,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2144,7 +2139,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J62">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2154,7 +2149,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J63">
-    <cfRule type="colorScale" priority="111">
+    <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2164,7 +2159,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56">
-    <cfRule type="colorScale" priority="116">
+    <cfRule type="colorScale" priority="117">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2174,6 +2169,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2183,8 +2188,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J41">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="I49:J54">
+    <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2193,28 +2198,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I57:J57">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I49:J54">
-    <cfRule type="colorScale" priority="122">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I58:J61">
-    <cfRule type="colorScale" priority="125">
+  <conditionalFormatting sqref="I57:J61">
+    <cfRule type="colorScale" priority="126">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2224,7 +2209,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:J47 J2:J12 H2:H63">
-    <cfRule type="colorScale" priority="127">
+    <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>